<commit_message>
FUNCTIONALITY: Updated statistics and removed an outdated an replaced test suite.
</commit_message>
<xml_diff>
--- a/QA/Tests/CRUD/Create/Step1/_Test_Suite_Statistics_for_Folders.xlsx
+++ b/QA/Tests/CRUD/Create/Step1/_Test_Suite_Statistics_for_Folders.xlsx
@@ -187,7 +187,7 @@
       <sheetData sheetId="0">
         <row r="1">
           <cell r="E1">
-            <v>9</v>
+            <v>3</v>
           </cell>
           <cell r="G1">
             <v>0</v>
@@ -195,17 +195,17 @@
         </row>
         <row r="2">
           <cell r="G2">
-            <v>7</v>
+            <v>3</v>
           </cell>
         </row>
         <row r="4">
           <cell r="G4">
-            <v>71</v>
+            <v>42</v>
           </cell>
         </row>
         <row r="5">
           <cell r="G5">
-            <v>59</v>
+            <v>42</v>
           </cell>
         </row>
       </sheetData>
@@ -228,7 +228,7 @@
       <sheetData sheetId="0">
         <row r="1">
           <cell r="E1">
-            <v>3</v>
+            <v>4</v>
           </cell>
           <cell r="G1">
             <v>0</v>
@@ -241,12 +241,12 @@
         </row>
         <row r="4">
           <cell r="G4">
-            <v>42</v>
+            <v>35</v>
           </cell>
         </row>
         <row r="5">
           <cell r="G5">
-            <v>42</v>
+            <v>30</v>
           </cell>
         </row>
       </sheetData>
@@ -547,7 +547,7 @@
   <dimension ref="A1:J174"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J2" sqref="J2"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -589,7 +589,7 @@
       </c>
       <c r="H1" s="4">
         <f>SUM($D:$D)</f>
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="I1" s="3"/>
     </row>
@@ -598,23 +598,23 @@
         <v>14</v>
       </c>
       <c r="B2" s="1">
-        <f>[2]Sheet1!$G$1</f>
+        <f>[1]Sheet1!$G$1</f>
         <v>0</v>
       </c>
       <c r="C2" s="1">
-        <f>[2]Sheet1!$G$2</f>
+        <f>[1]Sheet1!$G$2</f>
         <v>3</v>
       </c>
       <c r="D2" s="1">
-        <f>[2]Sheet1!$E$1</f>
+        <f>[1]Sheet1!$E$1</f>
         <v>3</v>
       </c>
       <c r="E2" s="1">
-        <f>[2]Sheet1!$G$5</f>
+        <f>[1]Sheet1!$G$5</f>
         <v>42</v>
       </c>
       <c r="F2" s="1">
-        <f>[2]Sheet1!$G$4</f>
+        <f>[1]Sheet1!$G$4</f>
         <v>42</v>
       </c>
       <c r="G2" s="4" t="s">
@@ -629,7 +629,7 @@
       </c>
       <c r="J2" s="3">
         <f>SUM(H2:H3)</f>
-        <v>10</v>
+        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
@@ -637,31 +637,31 @@
         <v>13</v>
       </c>
       <c r="B3" s="1">
-        <f>[1]Sheet1!$G$1</f>
+        <f>[2]Sheet1!$G$1</f>
         <v>0</v>
       </c>
       <c r="C3" s="1">
-        <f>[1]Sheet1!$G$2</f>
-        <v>7</v>
+        <f>[2]Sheet1!$G$2</f>
+        <v>3</v>
       </c>
       <c r="D3" s="1">
-        <f>[1]Sheet1!$E$1</f>
-        <v>9</v>
+        <f>[2]Sheet1!$E$1</f>
+        <v>4</v>
       </c>
       <c r="E3" s="1">
-        <f>[1]Sheet1!$G$5</f>
-        <v>59</v>
+        <f>[2]Sheet1!$G$5</f>
+        <v>30</v>
       </c>
       <c r="F3" s="1">
-        <f>[1]Sheet1!$G$4</f>
-        <v>71</v>
+        <f>[2]Sheet1!$G$4</f>
+        <v>35</v>
       </c>
       <c r="G3" s="4" t="s">
         <v>4</v>
       </c>
       <c r="H3" s="4">
         <f>SUM($C:$C)</f>
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="I3" s="3"/>
     </row>
@@ -676,7 +676,7 @@
       </c>
       <c r="H5" s="4">
         <f xml:space="preserve"> SUM($F:$F)</f>
-        <v>113</v>
+        <v>77</v>
       </c>
       <c r="I5" s="3"/>
     </row>
@@ -686,7 +686,7 @@
       </c>
       <c r="H6" s="4">
         <f xml:space="preserve"> SUM($E:$E)</f>
-        <v>101</v>
+        <v>72</v>
       </c>
       <c r="I6" s="3"/>
     </row>
@@ -696,7 +696,7 @@
       </c>
       <c r="H7" s="7">
         <f>H6/H5</f>
-        <v>0.89380530973451322</v>
+        <v>0.93506493506493504</v>
       </c>
       <c r="I7" s="3"/>
     </row>

</xml_diff>